<commit_message>
Revisi / Tambah Fitur
</commit_message>
<xml_diff>
--- a/Raw Database.xlsx
+++ b/Raw Database.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\arfan-sc-sistempakar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C0EB66-3EC2-4ED2-968F-9F07C56A3255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD20CD69-D807-46B1-9527-C4A490C8E85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDA3C305-69BD-429E-ADF0-872BABF9CDEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{DDA3C305-69BD-429E-ADF0-872BABF9CDEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Gejala" sheetId="2" r:id="rId2"/>
+    <sheet name="Pasien" sheetId="3" r:id="rId3"/>
+    <sheet name="Penyakit" sheetId="4" r:id="rId4"/>
+    <sheet name="Rule" sheetId="5" r:id="rId5"/>
+    <sheet name="gejala_pasien" sheetId="6" r:id="rId6"/>
+    <sheet name="hasil_diagnosa" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -58,6 +64,93 @@
   </si>
   <si>
     <t>avatar</t>
+  </si>
+  <si>
+    <t>id_gejala</t>
+  </si>
+  <si>
+    <t>kode_gejala</t>
+  </si>
+  <si>
+    <t>nama_gejala</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>id_pasien</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>nama_pasien</t>
+  </si>
+  <si>
+    <t>nik</t>
+  </si>
+  <si>
+    <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>tanggal_lahir</t>
+  </si>
+  <si>
+    <t>usia</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>no_hp</t>
+  </si>
+  <si>
+    <t>id_penyakit</t>
+  </si>
+  <si>
+    <t>nama_penyakit</t>
+  </si>
+  <si>
+    <t>deskripsi</t>
+  </si>
+  <si>
+    <t>solusi</t>
+  </si>
+  <si>
+    <t>id_aturan</t>
+  </si>
+  <si>
+    <t>nilai_md</t>
+  </si>
+  <si>
+    <t>nilai_mb</t>
+  </si>
+  <si>
+    <t>id_gejala_pasien</t>
+  </si>
+  <si>
+    <t>cf_user</t>
+  </si>
+  <si>
+    <t>id_hasil</t>
+  </si>
+  <si>
+    <t>tanggal_diagnosa</t>
+  </si>
+  <si>
+    <t>nilai_cf</t>
+  </si>
+  <si>
+    <t>diagnosa</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>kode_penyakit</t>
   </si>
 </sst>
 </file>
@@ -411,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873A9CED-E801-4905-AD12-96C2B37E109A}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -460,4 +553,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A79A5A4-FAAB-4A42-A5CE-147FC93C1540}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EED065F-143E-4F0B-856E-BAF06D954C83}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A617B634-0FCE-4D38-AB47-471B86A5FAD4}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B29F2D4-BB40-4FD1-9E58-2804C31C23F3}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94EE37A4-E2AA-464E-8DDC-0C16C99C71D0}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1AD1D1-80DC-4304-B17F-E3D65EF3C9B1}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>